<commit_message>
Update untuk tugas iot
</commit_message>
<xml_diff>
--- a/SEMESTER 1/METODE KOMPUTASI/Tugas 1-Metode Komputasi-Tobias Mikha S.xlsx
+++ b/SEMESTER 1/METODE KOMPUTASI/Tugas 1-Metode Komputasi-Tobias Mikha S.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobias.sulistiyo\Desktop\Pascasarjana\SEMESTER 1\METODE KOMPUTASI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\S2-Pascasarjana\SEMESTER 1\METODE KOMPUTASI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A4D83A-3033-4585-A1E5-AA2D46AEC884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Question" sheetId="5" r:id="rId1"/>
     <sheet name="Bisection" sheetId="6" r:id="rId2"/>
     <sheet name="False Position" sheetId="8" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="9" r:id="rId4"/>
-    <sheet name="Newthon Raphson" sheetId="3" r:id="rId5"/>
+    <sheet name="Newthon Raphson" sheetId="9" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Bracketing Methode Using Bisection method</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>f(xl)</t>
-  </si>
-  <si>
-    <t>667.38/xl</t>
   </si>
   <si>
     <t>1-e^-0,146843.xl</t>
@@ -77,16 +74,7 @@
     <t>1-e^-0,146843.xu</t>
   </si>
   <si>
-    <t>f(x)</t>
-  </si>
-  <si>
-    <t>f'(x)</t>
-  </si>
-  <si>
     <t>err</t>
-  </si>
-  <si>
-    <t>Using Newthon Raphson</t>
   </si>
   <si>
     <t xml:space="preserve">Xr =(xl+xu)/2 </t>
@@ -118,11 +106,23 @@
   <si>
     <t>xr = (xl+xu)/2</t>
   </si>
+  <si>
+    <t>Methode Newthon Raphson</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>g(x)</t>
+  </si>
+  <si>
+    <t>g'(x)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -329,37 +329,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -372,6 +347,37 @@
   </cellStyles>
   <dxfs count="38">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -387,8 +393,136 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -415,165 +549,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -625,30 +600,30 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -987,7 +962,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E8A9E10C-85A0-2798-E659-A6B6BD70A432}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1036,7 +1011,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E89FCFE7-B16E-BB35-5149-7A146F18BA35}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1085,7 +1060,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E89FCFE7-B16E-BB35-5149-7A146F18BA35}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1129,7 +1104,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4BC71BB7-4BEA-4096-BE5F-3F15311E2EF8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1162,23 +1137,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>705053</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>181049</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428827</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>123913</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CA5F0F88-1472-7F38-EF7E-F7608CA2EB86}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF9BBE5E-0967-44CE-ACFC-F9F8CDC8A012}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1194,8 +1169,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1076325" y="409575"/>
-          <a:ext cx="1457528" cy="533474"/>
+          <a:off x="5076825" y="447675"/>
+          <a:ext cx="1448002" cy="628738"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1206,23 +1181,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>819380</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>161981</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>490678</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66756</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FCB8DC3A-4FE7-1576-322A-4249A4A02589}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E09993AD-E5FD-447A-92D8-8DFA9946A0EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1238,52 +1213,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2600325" y="523875"/>
-          <a:ext cx="1648055" cy="400106"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>38302</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>85813</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BE4310AC-7070-5AC0-27B1-F19EBEB79726}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4381500" y="409575"/>
-          <a:ext cx="1448002" cy="628738"/>
+          <a:off x="1133475" y="438150"/>
+          <a:ext cx="3624403" cy="581106"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1296,43 +1227,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="B7:O19" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="B7:O19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table13" displayName="Table13" ref="B7:O19" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="B7:O19" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="i" dataDxfId="32"/>
-    <tableColumn id="2" name="xl" dataDxfId="31"/>
-    <tableColumn id="3" name="xu" dataDxfId="30"/>
-    <tableColumn id="5" name="xr = (xl+xu)/2" dataDxfId="29">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="i" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="xl" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="xu" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="xr = (xl+xu)/2" dataDxfId="29">
       <calculatedColumnFormula>(C8+D8)/2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="1/root(xl)" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="1/root(xl)" dataDxfId="28">
       <calculatedColumnFormula>1/SQRT(Table13[[#This Row],[xl]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="1-e^-0,146843.xl" dataDxfId="27">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="1-e^-0,146843.xl" dataDxfId="27">
       <calculatedColumnFormula>2*LOG((0.0000015/3.7*(0.005))+(2.51/13743*F8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="1/root(xu)" dataDxfId="26">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="1/root(xu)" dataDxfId="26">
       <calculatedColumnFormula>1/SQRT(Table13[[#This Row],[xu]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="1-e^-0,146843.xu" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="1-e^-0,146843.xu" dataDxfId="25">
       <calculatedColumnFormula>2*LOG((0.0000015/3.7*(0.005))+(2.51/13743*H8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="1/root(xr)" dataDxfId="24">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="1/root(xr)" dataDxfId="24">
       <calculatedColumnFormula>1/SQRT(Table13[[#This Row],[xr = (xl+xu)/2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="1-e^-0,146843.xr" dataDxfId="23">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="1-e^-0,146843.xr" dataDxfId="23">
       <calculatedColumnFormula>2*LOG((0.0000015/3.7*(0.005))+(2.51/13.743*J8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="f(xl)" dataDxfId="22">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="f(xl)" dataDxfId="22">
       <calculatedColumnFormula>Table13[[#This Row],[1/root(xl)]]+Table13[[#This Row],[1-e^-0,146843.xl]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="f(xu)" dataDxfId="21">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="f(xu)" dataDxfId="21">
       <calculatedColumnFormula>Table13[[#This Row],[1/root(xu)]]+Table13[[#This Row],[1-e^-0,146843.xu]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="f(xr)" dataDxfId="20">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="f(xr)" dataDxfId="20">
       <calculatedColumnFormula>Table13[[#This Row],[1/root(xr)]]+Table13[[#This Row],[1-e^-0,146843.xr]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="er(%)" dataDxfId="19">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="er(%)" dataDxfId="19">
       <calculatedColumnFormula>ABS((E8-E7)/E8)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1341,47 +1272,69 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="B7:O19" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
-  <autoFilter ref="B7:O19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table134" displayName="Table134" ref="B7:O19" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="B7:O19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="i" dataDxfId="13"/>
-    <tableColumn id="2" name="xl" dataDxfId="12"/>
-    <tableColumn id="3" name="xu" dataDxfId="11"/>
-    <tableColumn id="5" name="xr" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="i" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="xl" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="xu" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="xr" dataDxfId="10">
       <calculatedColumnFormula>Table134[[#This Row],[xu]]-((Table134[[#This Row],[f(xu)]]*(Table134[[#This Row],[xl]]-Table134[[#This Row],[xu]]))/(Table134[[#This Row],[f(xl)]]-Table134[[#This Row],[f(xu)]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="1/root(xl)" dataDxfId="10">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="1/root(xl)" dataDxfId="9">
       <calculatedColumnFormula>1/SQRT(Table134[[#This Row],[xl]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="1-e^-0,146843.xl" dataDxfId="9">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="1-e^-0,146843.xl" dataDxfId="8">
       <calculatedColumnFormula>2*LOG((0.0000015/3.7*(0.005))+(2.51/13743*F8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="1/root(xu)" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="1/root(xu)" dataDxfId="7">
       <calculatedColumnFormula>1/SQRT(Table134[[#This Row],[xu]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="1-e^-0,146843.xu" dataDxfId="7">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="1-e^-0,146843.xu" dataDxfId="6">
       <calculatedColumnFormula>2*LOG((0.0000015/3.7*(0.005))+(2.51/13743*H8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="1/root(xr)" dataDxfId="6">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0100-00000F000000}" name="1/root(xr)" dataDxfId="5">
       <calculatedColumnFormula>1/SQRT(Table134[[#This Row],[xr]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="1-e^-0,146843.xr" dataDxfId="0">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0100-00000E000000}" name="1-e^-0,146843.xr" dataDxfId="4">
       <calculatedColumnFormula>2*LOG((0.0000015/3.7*(0.005))+(2.51/13743*J8))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="f(xl)" dataDxfId="5">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="f(xl)" dataDxfId="3">
       <calculatedColumnFormula>Table134[[#This Row],[1/root(xl)]]+Table134[[#This Row],[1-e^-0,146843.xl]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="f(xu)" dataDxfId="4">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="f(xu)" dataDxfId="2">
       <calculatedColumnFormula>Table134[[#This Row],[1/root(xu)]]+Table134[[#This Row],[1-e^-0,146843.xu]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="f(xr)" dataDxfId="3">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0100-00000D000000}" name="f(xr)" dataDxfId="1">
       <calculatedColumnFormula>Table134[[#This Row],[1/root(xr)]]+Table134[[#This Row],[1-e^-0,146843.xr]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="er(%)" dataDxfId="2">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="er(%)" dataDxfId="0">
       <calculatedColumnFormula>ABS((E8-E7)/E8)*100</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C95367DE-31AF-41D4-A62E-7EB77C67CFE6}" name="Table1" displayName="Table1" ref="C8:G16" totalsRowShown="0">
+  <autoFilter ref="C8:G16" xr:uid="{C95367DE-31AF-41D4-A62E-7EB77C67CFE6}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2DC28E1C-BC55-4B74-AB2C-9E6254B2845C}" name="i"/>
+    <tableColumn id="2" xr3:uid="{A7271DA8-ADF3-4560-933B-EF585C2A91CB}" name="x">
+      <calculatedColumnFormula>D8 - E8/F8</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{D47C4E0E-B324-4E84-AD75-A20F7E5EC4EB}" name="g(x)">
+      <calculatedColumnFormula>1/SQRT(D9) + 2*LOG(0.0000015/(3.7*0.005) + 2.51/(13743*SQRT(D9)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{B077F06C-6491-4473-A222-CF995A082467}" name="g'(x)">
+      <calculatedColumnFormula>-(0.3653579493*D9^(3/2) + 0.1826384341*D9)/(0.3652768682*D9^(5/2) + 0.0001621622*D9^3)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{B9229337-5F97-4C64-9B2B-AC24C6FF0429}" name="err">
+      <calculatedColumnFormula>ABS((D9 - D8) / D9) * 100</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1681,10 +1634,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:B4"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -1692,12 +1645,12 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1707,7 +1660,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1737,7 +1690,7 @@
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
@@ -1745,43 +1698,43 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -1834,7 +1787,7 @@
         <v>4.8113129462279609</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -2167,7 +2120,7 @@
         <v>0.70810385523209263</v>
       </c>
     </row>
-    <row r="15" spans="2:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>8</v>
       </c>
@@ -2223,56 +2176,56 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="25">
+      <c r="B16" s="7">
         <v>9</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="8">
         <v>7.9718750000000005E-2</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="8">
         <v>0.08</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="16">
         <f t="shared" si="0"/>
         <v>7.985937500000001E-2</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="8">
         <f>1/SQRT(Table13[[#This Row],[xl]])</f>
         <v>3.5417651464775051</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="8">
         <f t="shared" si="1"/>
         <v>-6.378373408487831</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="8">
         <f>1/SQRT(Table13[[#This Row],[xu]])</f>
         <v>3.5355339059327378</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="8">
         <f t="shared" si="2"/>
         <v>-6.3799029103927758</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="8">
         <f>1/SQRT(Table13[[#This Row],[xr = (xl+xu)/2]])</f>
         <v>3.5386454114636554</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="8">
         <f t="shared" si="3"/>
         <v>-0.37914155427653051</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="8">
         <f>Table13[[#This Row],[1/root(xl)]]+Table13[[#This Row],[1-e^-0,146843.xl]]</f>
         <v>-2.8366082620103259</v>
       </c>
-      <c r="M16" s="26">
+      <c r="M16" s="8">
         <f>Table13[[#This Row],[1/root(xu)]]+Table13[[#This Row],[1-e^-0,146843.xu]]</f>
         <v>-2.844369004460038</v>
       </c>
-      <c r="N16" s="26">
+      <c r="N16" s="8">
         <f>Table13[[#This Row],[1/root(xr)]]+Table13[[#This Row],[1-e^-0,146843.xr]]</f>
         <v>3.1595038571871248</v>
       </c>
-      <c r="O16" s="28">
+      <c r="O16" s="9">
         <f t="shared" si="4"/>
         <v>0.17609078458228017</v>
       </c>
@@ -2333,7 +2286,7 @@
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="25">
+      <c r="B18" s="7">
         <v>11</v>
       </c>
       <c r="C18" s="8">
@@ -2346,39 +2299,39 @@
         <f t="shared" ref="E18:E19" si="5">(C18+D18)/2</f>
         <v>7.9964843750000014E-2</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="8">
         <f>1/SQRT(Table13[[#This Row],[xl]])</f>
         <v>3.5370886322753625</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="8">
         <f t="shared" si="1"/>
         <v>-6.3795210396173525</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="8">
         <f>1/SQRT(Table13[[#This Row],[xu]])</f>
         <v>3.5355339059327378</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="8">
         <f t="shared" si="2"/>
         <v>-6.3799029103927758</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="8">
         <f>1/SQRT(Table13[[#This Row],[xr = (xl+xu)/2]])</f>
         <v>3.5363110127803958</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="8">
         <f t="shared" si="3"/>
         <v>-0.37971474028052504</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="8">
         <f>Table13[[#This Row],[1/root(xl)]]+Table13[[#This Row],[1-e^-0,146843.xl]]</f>
         <v>-2.84243240734199</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="8">
         <f>Table13[[#This Row],[1/root(xu)]]+Table13[[#This Row],[1-e^-0,146843.xu]]</f>
         <v>-2.844369004460038</v>
       </c>
-      <c r="N18" s="20">
+      <c r="N18" s="9">
         <f>Table13[[#This Row],[1/root(xr)]]+Table13[[#This Row],[1-e^-0,146843.xr]]</f>
         <v>3.1565962724998706</v>
       </c>
@@ -2401,39 +2354,39 @@
         <f t="shared" si="5"/>
         <v>7.9982421875000015E-2</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="14">
         <f>1/SQRT(Table13[[#This Row],[xl]])</f>
         <v>3.5363110127803958</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="14">
         <f t="shared" si="1"/>
         <v>-6.3797120169771526</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="14">
         <f>1/SQRT(Table13[[#This Row],[xu]])</f>
         <v>3.5355339059327378</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="14">
         <f t="shared" si="2"/>
         <v>-6.3799029103927758</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="14">
         <f>1/SQRT(Table13[[#This Row],[xr = (xl+xu)/2]])</f>
         <v>3.5359223953108629</v>
       </c>
-      <c r="K19" s="21">
+      <c r="K19" s="14">
         <f t="shared" si="3"/>
         <v>-0.37981019777605191</v>
       </c>
-      <c r="L19" s="21">
+      <c r="L19" s="14">
         <f>Table13[[#This Row],[1/root(xl)]]+Table13[[#This Row],[1-e^-0,146843.xl]]</f>
         <v>-2.8434010041967568</v>
       </c>
-      <c r="M19" s="21">
+      <c r="M19" s="14">
         <f>Table13[[#This Row],[1/root(xu)]]+Table13[[#This Row],[1-e^-0,146843.xu]]</f>
         <v>-2.844369004460038</v>
       </c>
-      <c r="N19" s="22">
+      <c r="N19" s="15">
         <f>Table13[[#This Row],[1/root(xr)]]+Table13[[#This Row],[1-e^-0,146843.xr]]</f>
         <v>3.156112197534811</v>
       </c>
@@ -2452,10 +2405,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2477,7 +2430,7 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2486,43 +2439,43 @@
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
@@ -2576,7 +2529,7 @@
         <v>-2.0132800013219541</v>
       </c>
       <c r="O8" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
@@ -2909,151 +2862,151 @@
         <v>2.346725733284714</v>
       </c>
     </row>
-    <row r="15" spans="2:15" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" s="7">
         <v>8</v>
       </c>
-      <c r="C15" s="26">
+      <c r="C15" s="8">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D15" s="26">
+      <c r="D15" s="8">
         <v>2.9370843803536301E-2</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="16">
         <f>Table134[[#This Row],[xu]]-((Table134[[#This Row],[f(xu)]]*(Table134[[#This Row],[xl]]-Table134[[#This Row],[xu]]))/(Table134[[#This Row],[f(xl)]]-Table134[[#This Row],[f(xu)]]))</f>
         <v>2.897410868025186E-2</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="8">
         <f>1/SQRT(Table134[[#This Row],[xl]])</f>
         <v>11.180339887498949</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="8">
         <f t="shared" si="0"/>
         <v>-5.3799047747847686</v>
       </c>
-      <c r="H15" s="26">
+      <c r="H15" s="8">
         <f>1/SQRT(Table134[[#This Row],[xu]])</f>
         <v>5.8350124652954314</v>
       </c>
-      <c r="I15" s="26">
+      <c r="I15" s="8">
         <f t="shared" si="1"/>
         <v>-5.9447304215923191</v>
       </c>
-      <c r="J15" s="26">
+      <c r="J15" s="8">
         <f>1/SQRT(Table134[[#This Row],[xr]])</f>
         <v>5.874825314910689</v>
       </c>
-      <c r="K15" s="26">
+      <c r="K15" s="8">
         <f t="shared" si="2"/>
         <v>-5.9388240939148078</v>
       </c>
-      <c r="L15" s="26">
+      <c r="L15" s="8">
         <f>Table134[[#This Row],[1/root(xl)]]+Table134[[#This Row],[1-e^-0,146843.xl]]</f>
         <v>5.8004351127141804</v>
       </c>
-      <c r="M15" s="26">
+      <c r="M15" s="8">
         <f>Table134[[#This Row],[1/root(xu)]]+Table134[[#This Row],[1-e^-0,146843.xu]]</f>
         <v>-0.10971795629688774</v>
       </c>
-      <c r="N15" s="26">
+      <c r="N15" s="8">
         <f>Table134[[#This Row],[1/root(xr)]]+Table134[[#This Row],[1-e^-0,146843.xr]]</f>
         <v>-6.3998779004118767E-2</v>
       </c>
-      <c r="O15" s="28">
+      <c r="O15" s="9">
         <f t="shared" si="3"/>
         <v>1.3692746433123124</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="25">
+      <c r="B16" s="7">
         <v>9</v>
       </c>
       <c r="C16" s="8">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="8">
         <v>2.897410868025186E-2</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="16">
         <f>Table134[[#This Row],[xu]]-((Table134[[#This Row],[f(xu)]]*(Table134[[#This Row],[xl]]-Table134[[#This Row],[xu]]))/(Table134[[#This Row],[f(xl)]]-Table134[[#This Row],[f(xu)]]))</f>
         <v>2.8745217474208697E-2</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="8">
         <f>1/SQRT(Table134[[#This Row],[xl]])</f>
         <v>11.180339887498949</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="8">
         <f t="shared" si="0"/>
         <v>-5.3799047747847686</v>
       </c>
-      <c r="H16" s="26">
+      <c r="H16" s="8">
         <f>1/SQRT(Table134[[#This Row],[xu]])</f>
         <v>5.874825314910689</v>
       </c>
-      <c r="I16" s="26">
+      <c r="I16" s="8">
         <f t="shared" si="1"/>
         <v>-5.9388240939148078</v>
       </c>
-      <c r="J16" s="26">
+      <c r="J16" s="8">
         <f>1/SQRT(Table134[[#This Row],[xr]])</f>
         <v>5.8981688430273289</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="8">
         <f t="shared" si="2"/>
         <v>-5.9353796142914925</v>
       </c>
-      <c r="L16" s="26">
+      <c r="L16" s="8">
         <f>Table134[[#This Row],[1/root(xl)]]+Table134[[#This Row],[1-e^-0,146843.xl]]</f>
         <v>5.8004351127141804</v>
       </c>
-      <c r="M16" s="26">
+      <c r="M16" s="8">
         <f>Table134[[#This Row],[1/root(xu)]]+Table134[[#This Row],[1-e^-0,146843.xu]]</f>
         <v>-6.3998779004118767E-2</v>
       </c>
-      <c r="N16" s="26">
+      <c r="N16" s="8">
         <f>Table134[[#This Row],[1/root(xr)]]+Table134[[#This Row],[1-e^-0,146843.xr]]</f>
         <v>-3.7210771264163611E-2</v>
       </c>
-      <c r="O16" s="28">
+      <c r="O16" s="9">
         <f t="shared" si="3"/>
         <v>0.79627578482762751</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="23">
+      <c r="B17" s="19">
         <v>10</v>
       </c>
       <c r="C17" s="11">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="20">
         <v>2.8745217474208697E-2</v>
       </c>
-      <c r="E17" s="30">
+      <c r="E17" s="21">
         <f>Table134[[#This Row],[xu]]-((Table134[[#This Row],[f(xu)]]*(Table134[[#This Row],[xl]]-Table134[[#This Row],[xu]]))/(Table134[[#This Row],[f(xl)]]-Table134[[#This Row],[f(xu)]]))</f>
         <v>2.8612981713835368E-2</v>
       </c>
-      <c r="F17" s="24">
+      <c r="F17" s="20">
         <f>1/SQRT(Table134[[#This Row],[xl]])</f>
         <v>11.180339887498949</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="20">
         <f t="shared" si="0"/>
         <v>-5.3799047747847686</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="20">
         <f>1/SQRT(Table134[[#This Row],[xu]])</f>
         <v>5.8981688430273289</v>
       </c>
-      <c r="I17" s="24">
+      <c r="I17" s="20">
         <f t="shared" si="1"/>
         <v>-5.9353796142914925</v>
       </c>
-      <c r="J17" s="24">
+      <c r="J17" s="20">
         <f>1/SQRT(Table134[[#This Row],[xr]])</f>
         <v>5.9117824151218956</v>
       </c>
-      <c r="K17" s="24">
+      <c r="K17" s="20">
         <f t="shared" si="2"/>
         <v>-5.9333771366802726</v>
       </c>
@@ -3069,13 +3022,13 @@
         <f>Table134[[#This Row],[1/root(xr)]]+Table134[[#This Row],[1-e^-0,146843.xr]]</f>
         <v>-2.1594721558376939E-2</v>
       </c>
-      <c r="O17" s="31">
+      <c r="O17" s="22">
         <f t="shared" si="3"/>
         <v>0.46215302444130668</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="25">
+      <c r="B18" s="7">
         <v>11</v>
       </c>
       <c r="C18" s="8">
@@ -3088,39 +3041,39 @@
         <f>Table134[[#This Row],[xu]]-((Table134[[#This Row],[f(xu)]]*(Table134[[#This Row],[xl]]-Table134[[#This Row],[xu]]))/(Table134[[#This Row],[f(xl)]]-Table134[[#This Row],[f(xu)]]))</f>
         <v>2.8536525286563589E-2</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="8">
         <f>1/SQRT(Table134[[#This Row],[xl]])</f>
         <v>11.180339887498949</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="8">
         <f t="shared" si="0"/>
         <v>-5.3799047747847686</v>
       </c>
-      <c r="H18" s="19">
+      <c r="H18" s="8">
         <f>1/SQRT(Table134[[#This Row],[xu]])</f>
         <v>5.9117824151218956</v>
       </c>
-      <c r="I18" s="19">
+      <c r="I18" s="8">
         <f t="shared" si="1"/>
         <v>-5.9333771366802726</v>
       </c>
-      <c r="J18" s="19">
+      <c r="J18" s="8">
         <f>1/SQRT(Table134[[#This Row],[xr]])</f>
         <v>5.919696683095748</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="8">
         <f t="shared" si="2"/>
         <v>-5.9322151122385103</v>
       </c>
-      <c r="L18" s="19">
+      <c r="L18" s="8">
         <f>Table134[[#This Row],[1/root(xl)]]+Table134[[#This Row],[1-e^-0,146843.xl]]</f>
         <v>5.8004351127141804</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="8">
         <f>Table134[[#This Row],[1/root(xu)]]+Table134[[#This Row],[1-e^-0,146843.xu]]</f>
         <v>-2.1594721558376939E-2</v>
       </c>
-      <c r="N18" s="20">
+      <c r="N18" s="9">
         <f>Table134[[#This Row],[1/root(xr)]]+Table134[[#This Row],[1-e^-0,146843.xr]]</f>
         <v>-1.2518429142762244E-2</v>
       </c>
@@ -3143,39 +3096,39 @@
         <f>Table134[[#This Row],[xu]]-((Table134[[#This Row],[f(xu)]]*(Table134[[#This Row],[xl]]-Table134[[#This Row],[xu]]))/(Table134[[#This Row],[f(xl)]]-Table134[[#This Row],[f(xu)]]))</f>
         <v>2.8492299053756599E-2</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="14">
         <f>1/SQRT(Table134[[#This Row],[xl]])</f>
         <v>11.180339887498949</v>
       </c>
-      <c r="G19" s="21">
+      <c r="G19" s="14">
         <f t="shared" si="0"/>
         <v>-5.3799047747847686</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="14">
         <f>1/SQRT(Table134[[#This Row],[xu]])</f>
         <v>5.919696683095748</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="14">
         <f t="shared" si="1"/>
         <v>-5.9322151122385103</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="14">
         <f>1/SQRT(Table134[[#This Row],[xr]])</f>
         <v>5.9242892287348656</v>
       </c>
-      <c r="K19" s="21">
+      <c r="K19" s="14">
         <f t="shared" si="2"/>
         <v>-5.9315415168439225</v>
       </c>
-      <c r="L19" s="21">
+      <c r="L19" s="14">
         <f>Table134[[#This Row],[1/root(xl)]]+Table134[[#This Row],[1-e^-0,146843.xl]]</f>
         <v>5.8004351127141804</v>
       </c>
-      <c r="M19" s="21">
+      <c r="M19" s="14">
         <f>Table134[[#This Row],[1/root(xu)]]+Table134[[#This Row],[1-e^-0,146843.xu]]</f>
         <v>-1.2518429142762244E-2</v>
       </c>
-      <c r="N19" s="22">
+      <c r="N19" s="15">
         <f>Table134[[#This Row],[1/root(xr)]]+Table134[[#This Row],[1-e^-0,146843.xr]]</f>
         <v>-7.2522881090568703E-3</v>
       </c>
@@ -3194,529 +3147,208 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="C2:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U28"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="8" width="21.140625" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="T4" t="s">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E9">
+        <f>1/SQRT(D9) + 2*LOG(0.0000015/(3.7*0.005) + 2.51/(13743*SQRT(D9)))</f>
+        <v>5.8342565891436111</v>
+      </c>
+      <c r="F9">
+        <f>-(0.3653579493*D9^(3/2) + 0.1826384341*D9)/(0.3652768682*D9^(5/2) + 0.0001621622*D9^3)</f>
+        <v>-823.76627972933795</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f>D9 - E9/F9</f>
+        <v>1.5082417346653899E-2</v>
+      </c>
+      <c r="E10">
+        <f>1/SQRT(D10) + 2*LOG(0.0000015/(3.7*0.005) + 2.51/(13743*SQRT(D10)))</f>
+        <v>2.5334504235420345</v>
+      </c>
+      <c r="F10">
+        <f>-(0.3653579493*D10^(3/2) + 0.1826384341*D10)/(0.3652768682*D10^(5/2) + 0.0001621622*D10^3)</f>
+        <v>-336.2364730522014</v>
+      </c>
+      <c r="G10">
+        <f>ABS((D10 - D9) / D10) * 100</f>
+        <v>46.958104817495752</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ref="D11:D13" si="0">D10 - E10/F10</f>
+        <v>2.2617145511461621E-2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:E13" si="1">1/SQRT(D11) + 2*LOG(0.0000015/(3.7*0.005) + 2.51/(13743*SQRT(D11)))</f>
+        <v>0.87426300036163962</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F13" si="2">-(0.3653579493*D11^(3/2) + 0.1826384341*D11)/(0.3652768682*D11^(5/2) + 0.0001621622*D11^3)</f>
+        <v>-191.20993245890597</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G13" si="3">ABS((D11 - D10) / D11) * 100</f>
+        <v>33.314231280819108</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12">
         <v>3</v>
-      </c>
-      <c r="U4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="T5" t="e">
-        <f xml:space="preserve"> 667.38/C4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U5">
-        <f xml:space="preserve"> 1-EXP(-0.146843*C4)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="T7" t="s">
-        <v>3</v>
-      </c>
-      <c r="U7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="D8">
-        <f>EXP(-C8)-C8</f>
-        <v>0.98403191483706065</v>
-      </c>
-      <c r="E8">
-        <f>-EXP(-C8)-1</f>
-        <v>-1.9920319148370607</v>
-      </c>
-      <c r="F8">
-        <v>100</v>
-      </c>
-      <c r="T8" t="e">
-        <f xml:space="preserve"> 667.38/C5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U8">
-        <f xml:space="preserve"> 1-EXP(-0.146843*C5)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <f>C8-(D8/E8)</f>
-        <v>0.50198401075193122</v>
-      </c>
-      <c r="D9">
-        <f t="shared" ref="D9:D28" si="0">EXP(-C9)-C9</f>
-        <v>0.1033444785642943</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ref="E9:E28" si="1">-EXP(-C9)-1</f>
-        <v>-1.6053284893162254</v>
-      </c>
-      <c r="F9">
-        <f>ABS((C9-C8)/C9)*100</f>
-        <v>98.406323741663272</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <f t="shared" ref="C10:C28" si="2">C9-(D9/E9)</f>
-        <v>0.56635991839455513</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>1.2278302629078475E-3</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="1"/>
-        <v>-1.567587748657463</v>
-      </c>
-      <c r="F10">
-        <f t="shared" ref="F10:F28" si="3">ABS((C10-C9)/C10)*100</f>
-        <v>11.366607267178885</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" si="2"/>
-        <v>0.56714317934052727</v>
-      </c>
-      <c r="D11" s="1">
-        <f>EXP(-C11)-C11</f>
-        <v>1.7406144370291088E-7</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.567143353401971</v>
-      </c>
-      <c r="F11" s="1">
-        <f t="shared" si="3"/>
-        <v>0.13810638556614854</v>
-      </c>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978162</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>3.5527136788005009E-15</v>
+        <v>2.7189413223284241E-2</v>
       </c>
       <c r="E12">
         <f t="shared" si="1"/>
-        <v>-1.5671432904097853</v>
+        <v>0.21471901782509217</v>
       </c>
       <c r="F12">
-        <f>ABS((C12-C11)/C12)*100</f>
-        <v>1.9583984546319324E-5</v>
-      </c>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>5</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>-148.30082034344551</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>16.816353020472906</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
+        <v>4</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.8637274518507224E-2</v>
       </c>
       <c r="E13">
         <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
+        <v>3.8446226918064319E-2</v>
       </c>
       <c r="F13">
+        <f t="shared" si="2"/>
+        <v>-138.09142650611611</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="3"/>
-        <v>3.9151411764846085E-13</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14">
+        <v>5.0558627507910483</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:D16" si="4">D13 - E13/F13</f>
+        <v>2.8915685915150747E-2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14:E16" si="5">1/SQRT(D14) + 2*LOG(0.0000015/(3.7*0.005) + 2.51/(13743*SQRT(D14)))</f>
+        <v>6.0214838314580632E-3</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ref="F14:F16" si="6">-(0.3653579493*D14^(3/2) + 0.1826384341*D14)/(0.3652768682*D14^(5/2) + 0.0001621622*D14^3)</f>
+        <v>-136.26870680602306</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:G16" si="7">ABS((D14 - D13) / D14) * 100</f>
+        <v>0.96283863872530706</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
         <v>6</v>
       </c>
-      <c r="C14">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="D15" s="1">
+        <f t="shared" si="4"/>
+        <v>2.8959874224943907E-2</v>
+      </c>
+      <c r="E15" s="1">
+        <f t="shared" si="5"/>
+        <v>9.1659928802823032E-4</v>
+      </c>
+      <c r="F15" s="1">
+        <f t="shared" si="6"/>
+        <v>-135.98328842514985</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="7"/>
+        <v>0.15258460534023963</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16">
         <v>7</v>
       </c>
-      <c r="C15">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>8</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2.8966614753862155E-2</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
+        <f t="shared" si="5"/>
+        <v>1.3888367100278742E-4</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>9</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>10</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>11</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>12</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>13</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>14</v>
-      </c>
-      <c r="C22">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>15</v>
-      </c>
-      <c r="C23">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>16</v>
-      </c>
-      <c r="C24">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>17</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>18</v>
-      </c>
-      <c r="C26">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>19</v>
-      </c>
-      <c r="C27">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>20</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="2"/>
-        <v>0.56714329040978384</v>
-      </c>
-      <c r="D28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="1"/>
-        <v>-1.567143290409784</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>-135.93984255458614</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="7"/>
+        <v>2.3269991939078381E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>